<commit_message>
excel output match by column name and value
</commit_message>
<xml_diff>
--- a/src/main/resources/Sample.xlsx
+++ b/src/main/resources/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhammika Mahendra\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4917E43F-457D-4006-850F-91205B2E3E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB76820-C280-41DB-BBB4-B709EB550E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{26F10AD8-DBE0-43A6-9A75-31E2304ECF0D}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Age </t>
-  </si>
-  <si>
     <t>Place</t>
   </si>
   <si>
@@ -66,6 +63,21 @@
   </si>
   <si>
     <t>SF</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -437,67 +449,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F75E72D-813A-4F38-85F8-98BC48777E58}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>